<commit_message>
Code for generating the image
</commit_message>
<xml_diff>
--- a/Notebook.xlsx
+++ b/Notebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\ResearchProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E92E2E-9277-4F70-8B3B-60981788D9B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40FC378-2EC7-42E1-BDD0-87EFEADC04DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="77">
   <si>
     <t>Notes</t>
   </si>
@@ -268,9 +268,6 @@
     <t>10:00-14:00               Mar 19</t>
   </si>
   <si>
-    <t>2:00-4:00               Mar 20</t>
-  </si>
-  <si>
     <t>Create project.docx</t>
   </si>
   <si>
@@ -283,12 +280,6 @@
     <t>Created code to form the beginning of the pipeline</t>
   </si>
   <si>
-    <t>12:00-4:00                  Mar 21</t>
-  </si>
-  <si>
-    <t>2:00-3:00            Mar 22</t>
-  </si>
-  <si>
     <t>Meeting to discuss gridding techniques</t>
   </si>
   <si>
@@ -298,13 +289,25 @@
     <t xml:space="preserve">Coding </t>
   </si>
   <si>
-    <t>5:00-8:00                 Mar 22</t>
-  </si>
-  <si>
     <t>Continuing gridding code</t>
   </si>
   <si>
     <t xml:space="preserve">Progess on code </t>
+  </si>
+  <si>
+    <t>14:00-16:00               Mar 20</t>
+  </si>
+  <si>
+    <t>12:00-16:00                  Mar 21</t>
+  </si>
+  <si>
+    <t>14:00-15:00            Mar 22</t>
+  </si>
+  <si>
+    <t>17:00-20:00                 Mar 22</t>
+  </si>
+  <si>
+    <t>14:00-18:00                Mar 24</t>
   </si>
 </sst>
 </file>
@@ -465,16 +468,16 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFill="1" applyProtection="1">
       <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -803,7 +806,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -822,10 +825,10 @@
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11"/>
+      <c r="C1" s="12"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -835,10 +838,10 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="13"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1126,7 +1129,7 @@
         <v>43</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D17" s="4">
         <v>2</v>
@@ -1135,10 +1138,10 @@
         <v>19</v>
       </c>
       <c r="F17" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="10" t="s">
         <v>64</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1146,7 +1149,7 @@
         <v>59</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D18" s="4">
         <v>4</v>
@@ -1155,18 +1158,18 @@
         <v>19</v>
       </c>
       <c r="F18" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="13" t="s">
-        <v>69</v>
+      <c r="C19" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="D19" s="4">
         <v>1</v>
@@ -1175,18 +1178,18 @@
         <v>31</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D20" s="4">
         <v>3</v>
@@ -1195,30 +1198,30 @@
         <v>19</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>15</v>
+        <v>76</v>
+      </c>
+      <c r="D21" s="4">
+        <v>4</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated project for 7/May
</commit_message>
<xml_diff>
--- a/Notebook.xlsx
+++ b/Notebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\ResearchProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD37A6B5-3A4F-4E30-B49D-9EED83039FD2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6F32C1-5793-44CE-8571-9F828F8873CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="139">
   <si>
     <t>Notes</t>
   </si>
@@ -376,9 +376,6 @@
     <t>11:00-14:00                     Apr 6</t>
   </si>
   <si>
-    <t>Wrote the first version of the Abtract</t>
-  </si>
-  <si>
     <t>11:00-18:00                            Apr 8</t>
   </si>
   <si>
@@ -395,6 +392,110 @@
   </si>
   <si>
     <t>Work on project.docx</t>
+  </si>
+  <si>
+    <t>12:00-16:00               Apr 9</t>
+  </si>
+  <si>
+    <t>13:00-15:00           Apr 11</t>
+  </si>
+  <si>
+    <t>Discussed what is required for Mid-semester review</t>
+  </si>
+  <si>
+    <t>Notes on what is to be included</t>
+  </si>
+  <si>
+    <t>Coded an initial version of the iFFT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simple iFFT to be adapted </t>
+  </si>
+  <si>
+    <t>More progress on project</t>
+  </si>
+  <si>
+    <t>Literature review complete and most of methods done</t>
+  </si>
+  <si>
+    <t>9:00-12:00                      Apr 12</t>
+  </si>
+  <si>
+    <t>17:00-20:00          Apr 11</t>
+  </si>
+  <si>
+    <t>Project is ready for submission for mid-project review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:00-16:00             Apr 12 </t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>Final touches on mid project review</t>
+  </si>
+  <si>
+    <t>Wrote the first version of the Abstract</t>
+  </si>
+  <si>
+    <t>Submitting</t>
+  </si>
+  <si>
+    <t>14:00-15:00               May 1</t>
+  </si>
+  <si>
+    <t>Discuss the poster presentation</t>
+  </si>
+  <si>
+    <t>Last review on the project before sending it away for the mid project review, 
+this version that was sent off can be found as the project docx containing -At Mid Project review-</t>
+  </si>
+  <si>
+    <t>Collected ideas for what the poster should look like by 
+discussing with Murray and looking over posters from previous years</t>
+  </si>
+  <si>
+    <t>~4</t>
+  </si>
+  <si>
+    <t>Made progress on iFFT code</t>
+  </si>
+  <si>
+    <t>Looking into different ways of implementing the iFFT</t>
+  </si>
+  <si>
+    <t>10:00:15:00                  Apr 15</t>
+  </si>
+  <si>
+    <t>11:00-16:00</t>
+  </si>
+  <si>
+    <t>Finished implementation of iFFT</t>
+  </si>
+  <si>
+    <t>Have working code for an iFFT when using separate grids for the real and complex part of the numbers</t>
+  </si>
+  <si>
+    <t>11:00-16:00          Apr 18</t>
+  </si>
+  <si>
+    <t>15:00-22:00                Apr 22</t>
+  </si>
+  <si>
+    <t>~6</t>
+  </si>
+  <si>
+    <t>Implement different iFFT</t>
+  </si>
+  <si>
+    <t>Began work on a pipeline uses a complex data type, this will be comapared against the other pipelines</t>
+  </si>
+  <si>
+    <t>Finish work on second pipeline</t>
+  </si>
+  <si>
+    <t>Finished the second pipeline</t>
   </si>
 </sst>
 </file>
@@ -511,7 +612,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -559,6 +660,10 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="6" applyFill="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
       <protection locked="0"/>
@@ -567,8 +672,20 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="6" applyFill="1">
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -896,8 +1013,8 @@
   </sheetPr>
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -916,10 +1033,10 @@
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12"/>
+      <c r="C1" s="13"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -929,10 +1046,10 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="13"/>
+      <c r="C2" s="14"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1469,7 +1586,7 @@
         <v>19</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="G29" s="10" t="s">
         <v>73</v>
@@ -1480,7 +1597,7 @@
         <v>51</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D30" s="4">
         <v>7</v>
@@ -1489,10 +1606,10 @@
         <v>19</v>
       </c>
       <c r="F30" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G30" s="10" t="s">
         <v>101</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1500,7 +1617,7 @@
         <v>38</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D31" s="4">
         <v>4</v>
@@ -1509,215 +1626,215 @@
         <v>19</v>
       </c>
       <c r="F31" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="G31" s="10" t="s">
         <v>104</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>15</v>
+        <v>51</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D32" s="4">
+        <v>4</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>14</v>
+        <v>109</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>17</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" s="4">
+        <v>2</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>14</v>
+        <v>107</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>17</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>15</v>
+        <v>114</v>
+      </c>
+      <c r="D34" s="4">
+        <v>3</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>17</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>15</v>
+        <v>113</v>
+      </c>
+      <c r="D35" s="4">
+        <v>3</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F36" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G36" s="14" t="s">
-        <v>17</v>
+        <v>120</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" s="4">
+        <v>1</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="G36" s="18" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G37" s="14" t="s">
-        <v>17</v>
+        <v>125</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G38" s="14" t="s">
-        <v>17</v>
+        <v>132</v>
+      </c>
+      <c r="D38" s="4">
+        <v>5</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>12</v>
+        <v>133</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E39" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F39" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G39" s="14" t="s">
-        <v>17</v>
+        <v>134</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E40" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F40" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G40" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="D40" s="4">
+        <v>5</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E41" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F41" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G41" s="14" t="s">
-        <v>17</v>
+        <v>121</v>
+      </c>
+      <c r="D41" s="4">
+        <v>1</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="G41" s="18" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>12</v>
@@ -1725,19 +1842,19 @@
       <c r="D42" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E42" s="14" t="s">
+      <c r="E42" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F42" s="14" t="s">
+      <c r="F42" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G42" s="14" t="s">
+      <c r="G42" s="12" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="43" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>12</v>
@@ -1745,13 +1862,13 @@
       <c r="D43" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E43" s="14" t="s">
+      <c r="E43" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F43" s="14" t="s">
+      <c r="F43" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G43" s="14" t="s">
+      <c r="G43" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1765,13 +1882,13 @@
       <c r="D44" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E44" s="14" t="s">
+      <c r="E44" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F44" s="14" t="s">
+      <c r="F44" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G44" s="14" t="s">
+      <c r="G44" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1785,13 +1902,13 @@
       <c r="D45" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E45" s="14" t="s">
+      <c r="E45" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F45" s="14" t="s">
+      <c r="F45" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G45" s="14" t="s">
+      <c r="G45" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1805,13 +1922,13 @@
       <c r="D46" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E46" s="14" t="s">
+      <c r="E46" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F46" s="14" t="s">
+      <c r="F46" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G46" s="14" t="s">
+      <c r="G46" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1825,13 +1942,13 @@
       <c r="D47" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E47" s="14" t="s">
+      <c r="E47" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F47" s="14" t="s">
+      <c r="F47" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G47" s="14" t="s">
+      <c r="G47" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1845,13 +1962,13 @@
       <c r="D48" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E48" s="14" t="s">
+      <c r="E48" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F48" s="14" t="s">
+      <c r="F48" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G48" s="14" t="s">
+      <c r="G48" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1865,13 +1982,13 @@
       <c r="D49" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E49" s="14" t="s">
+      <c r="E49" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F49" s="14" t="s">
+      <c r="F49" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G49" s="14" t="s">
+      <c r="G49" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1885,13 +2002,13 @@
       <c r="D50" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E50" s="14" t="s">
+      <c r="E50" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F50" s="14" t="s">
+      <c r="F50" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G50" s="14" t="s">
+      <c r="G50" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1905,13 +2022,13 @@
       <c r="D51" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E51" s="14" t="s">
+      <c r="E51" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F51" s="14" t="s">
+      <c r="F51" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G51" s="14" t="s">
+      <c r="G51" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1925,13 +2042,13 @@
       <c r="D52" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E52" s="14" t="s">
+      <c r="E52" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F52" s="14" t="s">
+      <c r="F52" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G52" s="14" t="s">
+      <c r="G52" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1945,13 +2062,13 @@
       <c r="D53" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="14" t="s">
+      <c r="E53" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F53" s="14" t="s">
+      <c r="F53" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G53" s="14" t="s">
+      <c r="G53" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1965,13 +2082,13 @@
       <c r="D54" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E54" s="14" t="s">
+      <c r="E54" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F54" s="14" t="s">
+      <c r="F54" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G54" s="14" t="s">
+      <c r="G54" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1985,13 +2102,13 @@
       <c r="D55" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E55" s="14" t="s">
+      <c r="E55" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F55" s="14" t="s">
+      <c r="F55" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G55" s="14" t="s">
+      <c r="G55" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2005,13 +2122,13 @@
       <c r="D56" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E56" s="14" t="s">
+      <c r="E56" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F56" s="14" t="s">
+      <c r="F56" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G56" s="14" t="s">
+      <c r="G56" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2025,13 +2142,13 @@
       <c r="D57" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E57" s="14" t="s">
+      <c r="E57" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F57" s="14" t="s">
+      <c r="F57" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G57" s="14" t="s">
+      <c r="G57" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2045,13 +2162,13 @@
       <c r="D58" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E58" s="14" t="s">
+      <c r="E58" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F58" s="14" t="s">
+      <c r="F58" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G58" s="14" t="s">
+      <c r="G58" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2065,13 +2182,13 @@
       <c r="D59" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E59" s="14" t="s">
+      <c r="E59" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F59" s="14" t="s">
+      <c r="F59" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G59" s="14" t="s">
+      <c r="G59" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2085,13 +2202,13 @@
       <c r="D60" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E60" s="14" t="s">
+      <c r="E60" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F60" s="14" t="s">
+      <c r="F60" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G60" s="14" t="s">
+      <c r="G60" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2105,13 +2222,13 @@
       <c r="D61" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E61" s="14" t="s">
+      <c r="E61" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F61" s="14" t="s">
+      <c r="F61" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G61" s="14" t="s">
+      <c r="G61" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2125,13 +2242,13 @@
       <c r="D62" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E62" s="14" t="s">
+      <c r="E62" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F62" s="14" t="s">
+      <c r="F62" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G62" s="14" t="s">
+      <c r="G62" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2145,13 +2262,13 @@
       <c r="D63" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E63" s="14" t="s">
+      <c r="E63" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F63" s="14" t="s">
+      <c r="F63" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G63" s="14" t="s">
+      <c r="G63" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2165,13 +2282,13 @@
       <c r="D64" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E64" s="14" t="s">
+      <c r="E64" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F64" s="14" t="s">
+      <c r="F64" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G64" s="14" t="s">
+      <c r="G64" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2185,13 +2302,13 @@
       <c r="D65" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E65" s="14" t="s">
+      <c r="E65" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F65" s="14" t="s">
+      <c r="F65" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G65" s="14" t="s">
+      <c r="G65" s="12" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>